<commit_message>
Fixed some tree fire bugs.
</commit_message>
<xml_diff>
--- a/Documents+Tools/GAM_Project_Yarbus 2014-12-3.xlsx
+++ b/Documents+Tools/GAM_Project_Yarbus 2014-12-3.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="13272" windowHeight="7992" tabRatio="500" firstSheet="2" activeTab="9"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="13272" windowHeight="7992" tabRatio="500" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Game Data" sheetId="1" r:id="rId1"/>
@@ -4550,87 +4550,6 @@
     <xf numFmtId="10" fontId="5" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="155" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4658,16 +4577,94 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="155" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4677,15 +4674,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4709,20 +4697,20 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -4737,6 +4725,48 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="22" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="22" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4765,36 +4795,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="22" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="22" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -23755,51 +23755,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="147" t="s">
+      <c r="A1" s="120" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="148"/>
-      <c r="C1" s="148"/>
-      <c r="D1" s="149"/>
+      <c r="B1" s="121"/>
+      <c r="C1" s="121"/>
+      <c r="D1" s="122"/>
       <c r="E1" s="15"/>
-      <c r="F1" s="147" t="s">
+      <c r="F1" s="120" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="148"/>
-      <c r="H1" s="148"/>
-      <c r="I1" s="149"/>
+      <c r="G1" s="121"/>
+      <c r="H1" s="121"/>
+      <c r="I1" s="122"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
       <c r="L1" s="34"/>
     </row>
     <row r="2" spans="1:12" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="150" t="s">
+      <c r="A2" s="123" t="s">
         <v>899</v>
       </c>
-      <c r="B2" s="151"/>
-      <c r="C2" s="151"/>
-      <c r="D2" s="152"/>
+      <c r="B2" s="124"/>
+      <c r="C2" s="124"/>
+      <c r="D2" s="125"/>
       <c r="E2" s="15"/>
-      <c r="F2" s="150" t="s">
+      <c r="F2" s="123" t="s">
         <v>908</v>
       </c>
-      <c r="G2" s="151"/>
-      <c r="H2" s="151"/>
-      <c r="I2" s="152"/>
+      <c r="G2" s="124"/>
+      <c r="H2" s="124"/>
+      <c r="I2" s="125"/>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
       <c r="L2" s="34"/>
     </row>
     <row r="3" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="153"/>
-      <c r="B3" s="154"/>
-      <c r="C3" s="154"/>
-      <c r="D3" s="155"/>
+      <c r="A3" s="126"/>
+      <c r="B3" s="127"/>
+      <c r="C3" s="127"/>
+      <c r="D3" s="128"/>
       <c r="E3" s="15"/>
-      <c r="F3" s="153"/>
-      <c r="G3" s="154"/>
-      <c r="H3" s="154"/>
-      <c r="I3" s="155"/>
+      <c r="F3" s="126"/>
+      <c r="G3" s="127"/>
+      <c r="H3" s="127"/>
+      <c r="I3" s="128"/>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
       <c r="L3" s="34"/>
@@ -23819,93 +23819,93 @@
       <c r="L4" s="34"/>
     </row>
     <row r="5" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="147" t="s">
+      <c r="A5" s="120" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="148"/>
-      <c r="C5" s="148"/>
-      <c r="D5" s="149"/>
+      <c r="B5" s="121"/>
+      <c r="C5" s="121"/>
+      <c r="D5" s="122"/>
       <c r="E5" s="15"/>
-      <c r="F5" s="147" t="s">
+      <c r="F5" s="120" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="148"/>
-      <c r="H5" s="148"/>
-      <c r="I5" s="149"/>
+      <c r="G5" s="121"/>
+      <c r="H5" s="121"/>
+      <c r="I5" s="122"/>
       <c r="J5" s="5"/>
       <c r="K5" s="29"/>
       <c r="L5" s="34"/>
     </row>
     <row r="6" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="144" t="s">
+      <c r="A6" s="132" t="s">
         <v>909</v>
       </c>
-      <c r="B6" s="145"/>
-      <c r="C6" s="145"/>
-      <c r="D6" s="146"/>
+      <c r="B6" s="133"/>
+      <c r="C6" s="133"/>
+      <c r="D6" s="134"/>
       <c r="E6" s="15"/>
-      <c r="F6" s="144" t="s">
+      <c r="F6" s="132" t="s">
         <v>911</v>
       </c>
-      <c r="G6" s="145"/>
-      <c r="H6" s="145"/>
-      <c r="I6" s="146"/>
+      <c r="G6" s="133"/>
+      <c r="H6" s="133"/>
+      <c r="I6" s="134"/>
       <c r="J6" s="5"/>
-      <c r="K6" s="141" t="s">
+      <c r="K6" s="129" t="s">
         <v>28</v>
       </c>
       <c r="L6" s="34"/>
     </row>
     <row r="7" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="144" t="s">
+      <c r="A7" s="132" t="s">
         <v>910</v>
       </c>
-      <c r="B7" s="145"/>
-      <c r="C7" s="145"/>
-      <c r="D7" s="146"/>
+      <c r="B7" s="133"/>
+      <c r="C7" s="133"/>
+      <c r="D7" s="134"/>
       <c r="E7" s="15"/>
-      <c r="F7" s="144" t="s">
+      <c r="F7" s="132" t="s">
         <v>912</v>
       </c>
-      <c r="G7" s="145"/>
-      <c r="H7" s="145"/>
-      <c r="I7" s="146"/>
+      <c r="G7" s="133"/>
+      <c r="H7" s="133"/>
+      <c r="I7" s="134"/>
       <c r="J7" s="5"/>
-      <c r="K7" s="142"/>
+      <c r="K7" s="130"/>
       <c r="L7" s="34"/>
     </row>
     <row r="8" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="147" t="s">
+      <c r="A8" s="120" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="148"/>
-      <c r="C8" s="148"/>
-      <c r="D8" s="149"/>
+      <c r="B8" s="121"/>
+      <c r="C8" s="121"/>
+      <c r="D8" s="122"/>
       <c r="E8" s="15"/>
-      <c r="F8" s="144" t="s">
+      <c r="F8" s="132" t="s">
         <v>913</v>
       </c>
-      <c r="G8" s="145"/>
-      <c r="H8" s="145"/>
-      <c r="I8" s="146"/>
+      <c r="G8" s="133"/>
+      <c r="H8" s="133"/>
+      <c r="I8" s="134"/>
       <c r="J8" s="5"/>
-      <c r="K8" s="142"/>
+      <c r="K8" s="130"/>
       <c r="L8" s="34"/>
     </row>
     <row r="9" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="144"/>
-      <c r="B9" s="145"/>
-      <c r="C9" s="145"/>
-      <c r="D9" s="146"/>
+      <c r="A9" s="132"/>
+      <c r="B9" s="133"/>
+      <c r="C9" s="133"/>
+      <c r="D9" s="134"/>
       <c r="E9" s="15"/>
-      <c r="F9" s="144" t="s">
+      <c r="F9" s="132" t="s">
         <v>914</v>
       </c>
-      <c r="G9" s="145"/>
-      <c r="H9" s="145"/>
-      <c r="I9" s="146"/>
+      <c r="G9" s="133"/>
+      <c r="H9" s="133"/>
+      <c r="I9" s="134"/>
       <c r="J9" s="5"/>
-      <c r="K9" s="143"/>
+      <c r="K9" s="131"/>
       <c r="L9" s="34"/>
     </row>
     <row r="10" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -23923,17 +23923,17 @@
       <c r="L10" s="34"/>
     </row>
     <row r="11" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="147" t="s">
+      <c r="A11" s="120" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="148"/>
-      <c r="C11" s="148"/>
-      <c r="D11" s="149"/>
+      <c r="B11" s="121"/>
+      <c r="C11" s="121"/>
+      <c r="D11" s="122"/>
       <c r="E11" s="15"/>
-      <c r="F11" s="147" t="s">
+      <c r="F11" s="120" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="149"/>
+      <c r="G11" s="122"/>
       <c r="H11" s="2" t="s">
         <v>7</v>
       </c>
@@ -23972,7 +23972,7 @@
         <v>-0.14000000000000001</v>
       </c>
       <c r="J12" s="5"/>
-      <c r="K12" s="141" t="s">
+      <c r="K12" s="129" t="s">
         <v>8</v>
       </c>
       <c r="L12" s="34"/>
@@ -24002,7 +24002,7 @@
         <v>0</v>
       </c>
       <c r="J13" s="45"/>
-      <c r="K13" s="142"/>
+      <c r="K13" s="130"/>
       <c r="L13" s="46"/>
     </row>
     <row r="14" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -24029,7 +24029,7 @@
         <v>0</v>
       </c>
       <c r="J14" s="11"/>
-      <c r="K14" s="143"/>
+      <c r="K14" s="131"/>
       <c r="L14" s="50"/>
     </row>
     <row r="15" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -24089,10 +24089,10 @@
       </c>
       <c r="D17" s="44"/>
       <c r="E17" s="5"/>
-      <c r="F17" s="147" t="s">
+      <c r="F17" s="120" t="s">
         <v>16</v>
       </c>
-      <c r="G17" s="149"/>
+      <c r="G17" s="122"/>
       <c r="H17" s="2"/>
       <c r="I17" s="36">
         <v>0.75</v>
@@ -24116,16 +24116,16 @@
       <c r="F18" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="G18" s="125" t="s">
+      <c r="G18" s="135" t="s">
         <v>19</v>
       </c>
-      <c r="H18" s="127"/>
+      <c r="H18" s="136"/>
       <c r="I18" s="41">
         <f>IF(LEFT(G18,6)="Entire",0,IF(LEFT(G18,6)="Custom",-0.05,-0.1))</f>
         <v>0</v>
       </c>
       <c r="J18" s="52"/>
-      <c r="K18" s="141" t="s">
+      <c r="K18" s="129" t="s">
         <v>17</v>
       </c>
       <c r="L18" s="34"/>
@@ -24145,16 +24145,16 @@
       <c r="F19" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="G19" s="131" t="s">
+      <c r="G19" s="137" t="s">
         <v>21</v>
       </c>
-      <c r="H19" s="133"/>
+      <c r="H19" s="138"/>
       <c r="I19" s="49">
         <f>IF(G19="2D Graphics and 2D Gameplay",IF(I11=0.15,-0.05,0),IF(G19="3D Graphics but 2D Gameplay",IF(I11=0.15,-0.02,-0.3),IF(I11=0.15,0,-0.3)))</f>
         <v>0</v>
       </c>
       <c r="J19" s="5"/>
-      <c r="K19" s="143"/>
+      <c r="K19" s="131"/>
       <c r="L19" s="34"/>
     </row>
     <row r="20" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -24182,7 +24182,7 @@
       <c r="C21" s="43"/>
       <c r="D21" s="44"/>
       <c r="E21" s="5"/>
-      <c r="F21" s="138" t="s">
+      <c r="F21" s="153" t="s">
         <v>22</v>
       </c>
       <c r="G21" s="53"/>
@@ -24198,17 +24198,17 @@
       <c r="C22" s="43"/>
       <c r="D22" s="44"/>
       <c r="E22" s="5"/>
-      <c r="F22" s="139"/>
+      <c r="F22" s="154"/>
       <c r="G22" s="53"/>
       <c r="H22" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="I22" s="120">
+      <c r="I22" s="139">
         <f>I20+I15</f>
         <v>0.71</v>
       </c>
       <c r="J22" s="5"/>
-      <c r="K22" s="122" t="s">
+      <c r="K22" s="141" t="s">
         <v>25</v>
       </c>
       <c r="L22" s="34"/>
@@ -24219,14 +24219,14 @@
       <c r="C23" s="43"/>
       <c r="D23" s="44"/>
       <c r="E23" s="5"/>
-      <c r="F23" s="139"/>
+      <c r="F23" s="154"/>
       <c r="G23" s="53"/>
       <c r="H23" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="I23" s="121"/>
+      <c r="I23" s="140"/>
       <c r="J23" s="5"/>
-      <c r="K23" s="123"/>
+      <c r="K23" s="142"/>
       <c r="L23" s="34"/>
     </row>
     <row r="24" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -24235,7 +24235,7 @@
       <c r="C24" s="43"/>
       <c r="D24" s="44"/>
       <c r="E24" s="5"/>
-      <c r="F24" s="140"/>
+      <c r="F24" s="155"/>
       <c r="G24" s="53"/>
       <c r="H24" s="53"/>
       <c r="I24" s="53"/>
@@ -24263,12 +24263,12 @@
       <c r="C26" s="43"/>
       <c r="D26" s="44"/>
       <c r="E26" s="15"/>
-      <c r="F26" s="124" t="s">
+      <c r="F26" s="143" t="s">
         <v>26</v>
       </c>
-      <c r="G26" s="124"/>
-      <c r="H26" s="124"/>
-      <c r="I26" s="124"/>
+      <c r="G26" s="143"/>
+      <c r="H26" s="143"/>
+      <c r="I26" s="143"/>
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
       <c r="L26" s="34"/>
@@ -24279,12 +24279,12 @@
       <c r="C27" s="43"/>
       <c r="D27" s="44"/>
       <c r="E27" s="15"/>
-      <c r="F27" s="125" t="s">
+      <c r="F27" s="135" t="s">
         <v>27</v>
       </c>
-      <c r="G27" s="126"/>
-      <c r="H27" s="126"/>
-      <c r="I27" s="127"/>
+      <c r="G27" s="144"/>
+      <c r="H27" s="144"/>
+      <c r="I27" s="136"/>
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
       <c r="L27" s="34"/>
@@ -24295,10 +24295,10 @@
       <c r="C28" s="43"/>
       <c r="D28" s="44"/>
       <c r="E28" s="15"/>
-      <c r="F28" s="128"/>
-      <c r="G28" s="129"/>
-      <c r="H28" s="129"/>
-      <c r="I28" s="130"/>
+      <c r="F28" s="145"/>
+      <c r="G28" s="146"/>
+      <c r="H28" s="146"/>
+      <c r="I28" s="147"/>
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
       <c r="L28" s="34"/>
@@ -24309,10 +24309,10 @@
       <c r="C29" s="43"/>
       <c r="D29" s="44"/>
       <c r="E29" s="15"/>
-      <c r="F29" s="128"/>
-      <c r="G29" s="129"/>
-      <c r="H29" s="129"/>
-      <c r="I29" s="130"/>
+      <c r="F29" s="145"/>
+      <c r="G29" s="146"/>
+      <c r="H29" s="146"/>
+      <c r="I29" s="147"/>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
       <c r="L29" s="34"/>
@@ -24323,28 +24323,28 @@
       <c r="C30" s="43"/>
       <c r="D30" s="44"/>
       <c r="E30" s="15"/>
-      <c r="F30" s="128"/>
-      <c r="G30" s="129"/>
-      <c r="H30" s="129"/>
-      <c r="I30" s="130"/>
+      <c r="F30" s="145"/>
+      <c r="G30" s="146"/>
+      <c r="H30" s="146"/>
+      <c r="I30" s="147"/>
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
       <c r="L30" s="34"/>
     </row>
     <row r="31" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="134" t="s">
+      <c r="A31" s="149" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="135"/>
-      <c r="C31" s="136" t="s">
+      <c r="B31" s="150"/>
+      <c r="C31" s="151" t="s">
         <v>907</v>
       </c>
-      <c r="D31" s="137"/>
+      <c r="D31" s="152"/>
       <c r="E31" s="5"/>
-      <c r="F31" s="131"/>
-      <c r="G31" s="132"/>
-      <c r="H31" s="132"/>
-      <c r="I31" s="133"/>
+      <c r="F31" s="137"/>
+      <c r="G31" s="148"/>
+      <c r="H31" s="148"/>
+      <c r="I31" s="138"/>
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
       <c r="L31" s="34"/>
@@ -24365,12 +24365,13 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="A2:D3"/>
-    <mergeCell ref="F2:I3"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="K22:K23"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="F27:I31"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="F21:F24"/>
     <mergeCell ref="K12:K14"/>
     <mergeCell ref="K18:K19"/>
     <mergeCell ref="A6:D6"/>
@@ -24387,13 +24388,12 @@
     <mergeCell ref="G18:H18"/>
     <mergeCell ref="G19:H19"/>
     <mergeCell ref="A7:D7"/>
-    <mergeCell ref="I22:I23"/>
-    <mergeCell ref="K22:K23"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="F27:I31"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="F21:F24"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="A2:D3"/>
+    <mergeCell ref="F2:I3"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="F5:I5"/>
   </mergeCells>
   <dataValidations count="9">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A6:D7">
@@ -24441,7 +24441,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -24458,65 +24458,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="183" t="s">
+      <c r="A1" s="193" t="s">
         <v>700</v>
       </c>
       <c r="B1" s="73"/>
-      <c r="C1" s="198" t="s">
+      <c r="C1" s="183" t="s">
         <v>683</v>
       </c>
-      <c r="D1" s="199"/>
-      <c r="E1" s="198" t="s">
+      <c r="D1" s="184"/>
+      <c r="E1" s="183" t="s">
         <v>684</v>
       </c>
-      <c r="F1" s="199"/>
-      <c r="G1" s="198" t="s">
+      <c r="F1" s="184"/>
+      <c r="G1" s="183" t="s">
         <v>685</v>
       </c>
-      <c r="H1" s="199"/>
+      <c r="H1" s="184"/>
     </row>
     <row r="2" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="184"/>
+      <c r="A2" s="194"/>
       <c r="B2" s="73"/>
-      <c r="C2" s="200" t="s">
+      <c r="C2" s="185" t="s">
         <v>682</v>
       </c>
-      <c r="D2" s="201"/>
-      <c r="E2" s="200" t="s">
+      <c r="D2" s="186"/>
+      <c r="E2" s="185" t="s">
         <v>682</v>
       </c>
-      <c r="F2" s="201"/>
-      <c r="G2" s="200" t="s">
+      <c r="F2" s="186"/>
+      <c r="G2" s="185" t="s">
         <v>682</v>
       </c>
-      <c r="H2" s="201"/>
-      <c r="J2" s="186" t="s">
+      <c r="H2" s="186"/>
+      <c r="J2" s="196" t="s">
         <v>701</v>
       </c>
-      <c r="K2" s="187"/>
-      <c r="L2" s="188"/>
+      <c r="K2" s="197"/>
+      <c r="L2" s="198"/>
     </row>
     <row r="3" spans="1:12" ht="22.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="185"/>
+      <c r="A3" s="195"/>
       <c r="B3" s="74"/>
-      <c r="C3" s="196">
+      <c r="C3" s="187">
         <f>MAX(0,MIN(1,IF((A6+C6+L6) &lt;= 0.95, ROUND(A6+C6+L6,2), FLOOR((0.95+(A6+C6+L6-0.95)/5),0.01))))</f>
         <v>0.75</v>
       </c>
-      <c r="D3" s="197"/>
-      <c r="E3" s="196">
+      <c r="D3" s="188"/>
+      <c r="E3" s="187">
         <f>MAX(0,MIN(1,IF((A6+E6+L6) &lt;= 0.95, ROUND(A6+E6+L6,2), FLOOR((0.95+(A6+E6+L6-0.95)/5),0.01))))</f>
         <v>0.7</v>
       </c>
-      <c r="F3" s="197"/>
-      <c r="G3" s="196">
+      <c r="F3" s="188"/>
+      <c r="G3" s="187">
         <f>MAX(0,MIN(1,IF((A6+G6+L6) &lt;= 0.95, ROUND(A6+G6+L6,2), FLOOR((0.95+(A6+G6+L6-0.95)/5),0.01))))</f>
         <v>0.77</v>
       </c>
-      <c r="H3" s="197"/>
-      <c r="J3" s="189"/>
-      <c r="K3" s="190"/>
-      <c r="L3" s="191"/>
+      <c r="H3" s="188"/>
+      <c r="J3" s="199"/>
+      <c r="K3" s="200"/>
+      <c r="L3" s="201"/>
     </row>
     <row r="4" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
@@ -24536,18 +24536,18 @@
         <v>686</v>
       </c>
       <c r="B5" s="10"/>
-      <c r="C5" s="147" t="s">
+      <c r="C5" s="120" t="s">
         <v>687</v>
       </c>
-      <c r="D5" s="149"/>
-      <c r="E5" s="147" t="s">
+      <c r="D5" s="122"/>
+      <c r="E5" s="120" t="s">
         <v>688</v>
       </c>
-      <c r="F5" s="149"/>
-      <c r="G5" s="147" t="s">
+      <c r="F5" s="122"/>
+      <c r="G5" s="120" t="s">
         <v>689</v>
       </c>
-      <c r="H5" s="149"/>
+      <c r="H5" s="122"/>
       <c r="J5" s="75" t="s">
         <v>702</v>
       </c>
@@ -24562,21 +24562,21 @@
         <v>0.71</v>
       </c>
       <c r="B6" s="10"/>
-      <c r="C6" s="193">
+      <c r="C6" s="190">
         <f>D15+D24+D33+D42+D51+D60</f>
         <v>4.2499999999999996E-2</v>
       </c>
-      <c r="D6" s="194"/>
-      <c r="E6" s="193">
+      <c r="D6" s="191"/>
+      <c r="E6" s="190">
         <f>F15+F24+F33+F42+F51+F60</f>
         <v>-1.4999999999999972E-2</v>
       </c>
-      <c r="F6" s="194"/>
-      <c r="G6" s="193">
+      <c r="F6" s="191"/>
+      <c r="G6" s="190">
         <f>H15+H24+H33+H42+H51+H60</f>
         <v>5.7499999999999996E-2</v>
       </c>
-      <c r="H6" s="194"/>
+      <c r="H6" s="191"/>
       <c r="J6" s="90">
         <f>ABS('Student Grade'!$F$15+'Student Grade'!$D$24+'Student Grade'!$H$33+'Student Grade'!$F$42+'Student Grade'!$F$51+'Student Grade'!$F$60-$F$15-$D$24-$D$33-$H$42-$F$51-$F$60)</f>
         <v>0.1875</v>
@@ -24590,18 +24590,18 @@
     <row r="7" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
       <c r="B7" s="10"/>
-      <c r="C7" s="195" t="s">
+      <c r="C7" s="192" t="s">
         <v>690</v>
       </c>
-      <c r="D7" s="195"/>
-      <c r="E7" s="195" t="s">
+      <c r="D7" s="192"/>
+      <c r="E7" s="192" t="s">
         <v>691</v>
       </c>
-      <c r="F7" s="195"/>
-      <c r="G7" s="195" t="s">
+      <c r="F7" s="192"/>
+      <c r="G7" s="192" t="s">
         <v>692</v>
       </c>
-      <c r="H7" s="195"/>
+      <c r="H7" s="192"/>
       <c r="J7" s="89"/>
       <c r="K7" s="3"/>
       <c r="L7" s="87"/>
@@ -24775,7 +24775,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J12" s="141" t="s">
+      <c r="J12" s="129" t="s">
         <v>715</v>
       </c>
       <c r="K12" s="30"/>
@@ -24813,7 +24813,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J13" s="142"/>
+      <c r="J13" s="130"/>
       <c r="K13" s="30"/>
       <c r="L13" s="102" t="s">
         <v>708</v>
@@ -24849,7 +24849,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J14" s="142"/>
+      <c r="J14" s="130"/>
       <c r="K14" s="103"/>
       <c r="L14" s="102" t="s">
         <v>709</v>
@@ -24879,7 +24879,7 @@
         <f>SUM(H9:H14)</f>
         <v>-5.0000000000000001E-3</v>
       </c>
-      <c r="J15" s="142"/>
+      <c r="J15" s="130"/>
       <c r="K15" s="103"/>
       <c r="L15" s="102" t="s">
         <v>710</v>
@@ -24888,19 +24888,19 @@
     <row r="16" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
       <c r="B16" s="10"/>
-      <c r="C16" s="192" t="s">
+      <c r="C16" s="189" t="s">
         <v>690</v>
       </c>
-      <c r="D16" s="192"/>
-      <c r="E16" s="192" t="s">
+      <c r="D16" s="189"/>
+      <c r="E16" s="189" t="s">
         <v>691</v>
       </c>
-      <c r="F16" s="192"/>
-      <c r="G16" s="192" t="s">
+      <c r="F16" s="189"/>
+      <c r="G16" s="189" t="s">
         <v>692</v>
       </c>
-      <c r="H16" s="192"/>
-      <c r="J16" s="142"/>
+      <c r="H16" s="189"/>
+      <c r="J16" s="130"/>
       <c r="K16" s="103"/>
       <c r="L16" s="102" t="s">
         <v>711</v>
@@ -24931,7 +24931,7 @@
       <c r="H17" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="J17" s="142"/>
+      <c r="J17" s="130"/>
       <c r="K17" s="103"/>
       <c r="L17" s="102" t="s">
         <v>712</v>
@@ -24967,7 +24967,7 @@
         <f>B18*G18</f>
         <v>-0.05</v>
       </c>
-      <c r="J18" s="142"/>
+      <c r="J18" s="130"/>
       <c r="K18" s="103"/>
       <c r="L18" s="102" t="s">
         <v>713</v>
@@ -25003,7 +25003,7 @@
         <f t="shared" ref="H19:H23" si="5">B19*G19</f>
         <v>-0.01</v>
       </c>
-      <c r="J19" s="143"/>
+      <c r="J19" s="131"/>
       <c r="K19" s="103"/>
       <c r="L19" s="101" t="s">
         <v>714</v>
@@ -25161,18 +25161,18 @@
     <row r="25" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="3"/>
       <c r="B25" s="10"/>
-      <c r="C25" s="192" t="s">
+      <c r="C25" s="189" t="s">
         <v>690</v>
       </c>
-      <c r="D25" s="192"/>
-      <c r="E25" s="192" t="s">
+      <c r="D25" s="189"/>
+      <c r="E25" s="189" t="s">
         <v>691</v>
       </c>
-      <c r="F25" s="192"/>
-      <c r="G25" s="192" t="s">
+      <c r="F25" s="189"/>
+      <c r="G25" s="189" t="s">
         <v>692</v>
       </c>
-      <c r="H25" s="192"/>
+      <c r="H25" s="189"/>
     </row>
     <row r="26" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
@@ -25414,18 +25414,18 @@
     <row r="34" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="3"/>
       <c r="B34" s="10"/>
-      <c r="C34" s="192" t="s">
+      <c r="C34" s="189" t="s">
         <v>690</v>
       </c>
-      <c r="D34" s="192"/>
-      <c r="E34" s="192" t="s">
+      <c r="D34" s="189"/>
+      <c r="E34" s="189" t="s">
         <v>691</v>
       </c>
-      <c r="F34" s="192"/>
-      <c r="G34" s="192" t="s">
+      <c r="F34" s="189"/>
+      <c r="G34" s="189" t="s">
         <v>692</v>
       </c>
-      <c r="H34" s="192"/>
+      <c r="H34" s="189"/>
     </row>
     <row r="35" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
@@ -25667,18 +25667,18 @@
     <row r="43" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="3"/>
       <c r="B43" s="10"/>
-      <c r="C43" s="192" t="s">
+      <c r="C43" s="189" t="s">
         <v>690</v>
       </c>
-      <c r="D43" s="192"/>
-      <c r="E43" s="192" t="s">
+      <c r="D43" s="189"/>
+      <c r="E43" s="189" t="s">
         <v>691</v>
       </c>
-      <c r="F43" s="192"/>
-      <c r="G43" s="192" t="s">
+      <c r="F43" s="189"/>
+      <c r="G43" s="189" t="s">
         <v>692</v>
       </c>
-      <c r="H43" s="192"/>
+      <c r="H43" s="189"/>
     </row>
     <row r="44" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
@@ -25920,18 +25920,18 @@
     <row r="52" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="3"/>
       <c r="B52" s="10"/>
-      <c r="C52" s="192" t="s">
+      <c r="C52" s="189" t="s">
         <v>690</v>
       </c>
-      <c r="D52" s="192"/>
-      <c r="E52" s="192" t="s">
+      <c r="D52" s="189"/>
+      <c r="E52" s="189" t="s">
         <v>691</v>
       </c>
-      <c r="F52" s="192"/>
-      <c r="G52" s="192" t="s">
+      <c r="F52" s="189"/>
+      <c r="G52" s="189" t="s">
         <v>692</v>
       </c>
-      <c r="H52" s="192"/>
+      <c r="H52" s="189"/>
     </row>
     <row r="53" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
@@ -26172,27 +26172,6 @@
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:H16"/>
     <mergeCell ref="C52:D52"/>
     <mergeCell ref="E52:F52"/>
     <mergeCell ref="G52:H52"/>
@@ -26209,6 +26188,27 @@
     <mergeCell ref="E43:F43"/>
     <mergeCell ref="G43:H43"/>
     <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -26224,8 +26224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24:F24"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="13.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -26240,54 +26240,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="160" t="s">
+      <c r="A1" s="159" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="161"/>
-      <c r="C1" s="161"/>
-      <c r="D1" s="161"/>
-      <c r="E1" s="161"/>
-      <c r="F1" s="162"/>
+      <c r="B1" s="160"/>
+      <c r="C1" s="160"/>
+      <c r="D1" s="160"/>
+      <c r="E1" s="160"/>
+      <c r="F1" s="161"/>
     </row>
     <row r="2" spans="1:6" ht="43.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="163" t="s">
+      <c r="A2" s="156" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="164"/>
-      <c r="C2" s="164"/>
-      <c r="D2" s="164"/>
-      <c r="E2" s="164"/>
-      <c r="F2" s="165"/>
+      <c r="B2" s="157"/>
+      <c r="C2" s="157"/>
+      <c r="D2" s="157"/>
+      <c r="E2" s="157"/>
+      <c r="F2" s="158"/>
     </row>
     <row r="3" spans="1:6" ht="43.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="166" t="s">
+      <c r="A3" s="162" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="167"/>
-      <c r="C3" s="167"/>
-      <c r="D3" s="167"/>
-      <c r="E3" s="167"/>
-      <c r="F3" s="168"/>
+      <c r="B3" s="163"/>
+      <c r="C3" s="163"/>
+      <c r="D3" s="163"/>
+      <c r="E3" s="163"/>
+      <c r="F3" s="164"/>
     </row>
     <row r="4" spans="1:6" ht="28.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="163" t="s">
+      <c r="A4" s="156" t="s">
         <v>719</v>
       </c>
-      <c r="B4" s="164"/>
-      <c r="C4" s="164"/>
-      <c r="D4" s="164"/>
-      <c r="E4" s="164"/>
-      <c r="F4" s="165"/>
+      <c r="B4" s="157"/>
+      <c r="C4" s="157"/>
+      <c r="D4" s="157"/>
+      <c r="E4" s="157"/>
+      <c r="F4" s="158"/>
     </row>
     <row r="5" spans="1:6" ht="28.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="169" t="s">
+      <c r="A5" s="165" t="s">
         <v>62</v>
       </c>
-      <c r="B5" s="170"/>
-      <c r="C5" s="170"/>
-      <c r="D5" s="170"/>
-      <c r="E5" s="170"/>
-      <c r="F5" s="171"/>
+      <c r="B5" s="166"/>
+      <c r="C5" s="166"/>
+      <c r="D5" s="166"/>
+      <c r="E5" s="166"/>
+      <c r="F5" s="167"/>
     </row>
     <row r="6" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5"/>
@@ -26316,10 +26316,10 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="166" t="s">
+      <c r="A8" s="162" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="167"/>
+      <c r="B8" s="163"/>
       <c r="C8" s="16">
         <v>0</v>
       </c>
@@ -26335,10 +26335,10 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="156" t="s">
+      <c r="A9" s="169" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="157"/>
+      <c r="B9" s="170"/>
       <c r="C9" s="11">
         <v>0</v>
       </c>
@@ -26354,10 +26354,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="173" t="s">
+      <c r="A10" s="171" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="173"/>
+      <c r="B10" s="171"/>
       <c r="C10" s="11">
         <v>0</v>
       </c>
@@ -26373,10 +26373,10 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="173" t="s">
+      <c r="A11" s="171" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="173"/>
+      <c r="B11" s="171"/>
       <c r="C11" s="11">
         <v>0</v>
       </c>
@@ -26392,10 +26392,10 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="173" t="s">
+      <c r="A12" s="171" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="173"/>
+      <c r="B12" s="171"/>
       <c r="C12" s="11">
         <v>0</v>
       </c>
@@ -26411,10 +26411,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="156" t="s">
+      <c r="A13" s="169" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="157"/>
+      <c r="B13" s="170"/>
       <c r="C13" s="11">
         <v>0</v>
       </c>
@@ -26430,10 +26430,10 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="156" t="s">
+      <c r="A14" s="169" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="157"/>
+      <c r="B14" s="170"/>
       <c r="C14" s="11">
         <v>0</v>
       </c>
@@ -26449,10 +26449,10 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="158" t="s">
+      <c r="A15" s="172" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="159"/>
+      <c r="B15" s="173"/>
       <c r="C15" s="18">
         <v>0</v>
       </c>
@@ -26469,11 +26469,11 @@
     </row>
     <row r="16" spans="1:6" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
-      <c r="B16" s="172" t="s">
+      <c r="B16" s="168" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="172"/>
-      <c r="D16" s="172"/>
+      <c r="C16" s="168"/>
+      <c r="D16" s="168"/>
       <c r="E16" s="106">
         <f>SUM(E8:E15)</f>
         <v>0</v>
@@ -26492,88 +26492,93 @@
       <c r="A18" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="B18" s="160" t="s">
+      <c r="B18" s="159" t="s">
         <v>51</v>
       </c>
-      <c r="C18" s="161"/>
-      <c r="D18" s="161"/>
-      <c r="E18" s="161"/>
-      <c r="F18" s="162"/>
+      <c r="C18" s="160"/>
+      <c r="D18" s="160"/>
+      <c r="E18" s="160"/>
+      <c r="F18" s="161"/>
     </row>
     <row r="19" spans="1:6" ht="28.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="B19" s="163" t="s">
+      <c r="B19" s="156" t="s">
         <v>68</v>
       </c>
-      <c r="C19" s="164"/>
-      <c r="D19" s="164"/>
-      <c r="E19" s="164"/>
-      <c r="F19" s="165"/>
+      <c r="C19" s="157"/>
+      <c r="D19" s="157"/>
+      <c r="E19" s="157"/>
+      <c r="F19" s="158"/>
     </row>
     <row r="20" spans="1:6" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="62" t="s">
         <v>56</v>
       </c>
-      <c r="B20" s="163" t="s">
+      <c r="B20" s="156" t="s">
         <v>64</v>
       </c>
-      <c r="C20" s="164"/>
-      <c r="D20" s="164"/>
-      <c r="E20" s="164"/>
-      <c r="F20" s="165"/>
+      <c r="C20" s="157"/>
+      <c r="D20" s="157"/>
+      <c r="E20" s="157"/>
+      <c r="F20" s="158"/>
     </row>
     <row r="21" spans="1:6" ht="28.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="62" t="s">
         <v>57</v>
       </c>
-      <c r="B21" s="163" t="s">
+      <c r="B21" s="156" t="s">
         <v>65</v>
       </c>
-      <c r="C21" s="164"/>
-      <c r="D21" s="164"/>
-      <c r="E21" s="164"/>
-      <c r="F21" s="165"/>
+      <c r="C21" s="157"/>
+      <c r="D21" s="157"/>
+      <c r="E21" s="157"/>
+      <c r="F21" s="158"/>
     </row>
     <row r="22" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="62" t="s">
         <v>59</v>
       </c>
-      <c r="B22" s="163" t="s">
+      <c r="B22" s="156" t="s">
         <v>66</v>
       </c>
-      <c r="C22" s="164"/>
-      <c r="D22" s="164"/>
-      <c r="E22" s="164"/>
-      <c r="F22" s="165"/>
+      <c r="C22" s="157"/>
+      <c r="D22" s="157"/>
+      <c r="E22" s="157"/>
+      <c r="F22" s="158"/>
     </row>
     <row r="23" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="62" t="s">
         <v>58</v>
       </c>
-      <c r="B23" s="163" t="s">
+      <c r="B23" s="156" t="s">
         <v>60</v>
       </c>
-      <c r="C23" s="164"/>
-      <c r="D23" s="164"/>
-      <c r="E23" s="164"/>
-      <c r="F23" s="165"/>
+      <c r="C23" s="157"/>
+      <c r="D23" s="157"/>
+      <c r="E23" s="157"/>
+      <c r="F23" s="158"/>
     </row>
     <row r="24" spans="1:6" ht="43.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="62" t="s">
         <v>55</v>
       </c>
-      <c r="B24" s="163" t="s">
+      <c r="B24" s="156" t="s">
         <v>63</v>
       </c>
-      <c r="C24" s="164"/>
-      <c r="D24" s="164"/>
-      <c r="E24" s="164"/>
-      <c r="F24" s="165"/>
+      <c r="C24" s="157"/>
+      <c r="D24" s="157"/>
+      <c r="E24" s="157"/>
+      <c r="F24" s="158"/>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="B19:F19"/>
     <mergeCell ref="B24:F24"/>
     <mergeCell ref="B20:F20"/>
     <mergeCell ref="A1:F1"/>
@@ -26590,11 +26595,6 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="B19:F19"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -26610,7 +26610,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F126"/>
   <sheetViews>
-    <sheetView topLeftCell="A93" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="B117" sqref="B117"/>
     </sheetView>
   </sheetViews>
@@ -26653,7 +26653,7 @@
       <c r="B2" s="58" t="s">
         <v>74</v>
       </c>
-      <c r="C2" s="178" t="s">
+      <c r="C2" s="174" t="s">
         <v>878</v>
       </c>
       <c r="D2" s="64">
@@ -26676,7 +26676,7 @@
       <c r="B3" s="58" t="s">
         <v>76</v>
       </c>
-      <c r="C3" s="179"/>
+      <c r="C3" s="175"/>
       <c r="D3" s="64">
         <f>SUMPRODUCT(($A$10:$A$250="Basic")*(D$10:D$250="Missing"))+0.5*SUMPRODUCT(($A$10:$A$250="Basic")*(D$10:D$250="Partial"))</f>
         <v>0</v>
@@ -26697,7 +26697,7 @@
       <c r="B4" s="58" t="s">
         <v>78</v>
       </c>
-      <c r="C4" s="179"/>
+      <c r="C4" s="175"/>
       <c r="D4" s="64">
         <f>SUMPRODUCT(($A$10:$A$250="Intermediate")*(D$10:D$250="Missing"))+0.5*SUMPRODUCT(($A$10:$A$250="Intermediate")*(D$10:D$250="Partial"))</f>
         <v>0</v>
@@ -26718,7 +26718,7 @@
       <c r="B5" s="58" t="s">
         <v>80</v>
       </c>
-      <c r="C5" s="179"/>
+      <c r="C5" s="175"/>
       <c r="D5" s="64">
         <f>SUMPRODUCT(($A$10:$A$250="Intermediate")*(D$10:D$250="Completed"))+SUMPRODUCT(($A$10:$A$250="Intermediate")*(D$10:D$250="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$250="Intermediate")*(D$10:D$250="Partial"))</f>
         <v>18</v>
@@ -26739,7 +26739,7 @@
       <c r="B6" s="58" t="s">
         <v>82</v>
       </c>
-      <c r="C6" s="179"/>
+      <c r="C6" s="175"/>
       <c r="D6" s="64">
         <f>SUMPRODUCT(($A$10:$A$250="Advanced")*(D$10:D$250="Missing"))+0.5*SUMPRODUCT(($A$10:$A$250="Advanced")*(D$10:D$250="Partial"))</f>
         <v>1</v>
@@ -26760,7 +26760,7 @@
       <c r="B7" s="58" t="s">
         <v>84</v>
       </c>
-      <c r="C7" s="179"/>
+      <c r="C7" s="175"/>
       <c r="D7" s="64">
         <f>SUMPRODUCT(($A$10:$A$250="Advanced")*(D$10:D$250="Completed"))+SUMPRODUCT(($A$10:$A$250="Advanced")*(D$10:D$250="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$250="Advanced")*(D$10:D$250="Partial"))</f>
         <v>7</v>
@@ -26781,7 +26781,7 @@
       <c r="B8" s="58" t="s">
         <v>86</v>
       </c>
-      <c r="C8" s="179"/>
+      <c r="C8" s="175"/>
       <c r="D8" s="64">
         <f>SUMPRODUCT(($A$10:$A$250="Professional")*(D$10:D$250="Completed"))+SUMPRODUCT(($A$10:$A$250="Professional")*(D$10:D$250="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$250="Professional")*(D$10:D$250="Partial"))</f>
         <v>0</v>
@@ -26796,11 +26796,11 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="181" t="s">
+      <c r="A9" s="177" t="s">
         <v>87</v>
       </c>
-      <c r="B9" s="182"/>
-      <c r="C9" s="180"/>
+      <c r="B9" s="178"/>
+      <c r="C9" s="176"/>
       <c r="D9" s="64">
         <f>SUMPRODUCT(($A$10:$A$250="Innovative")*(D$10:D$250="Completed"))+SUMPRODUCT(($A$10:$A$250="Innovative")*(D$10:D$250="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$250="Innovative")*(D$10:D$250="Partial"))</f>
         <v>0</v>
@@ -26815,10 +26815,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="174" t="s">
+      <c r="A10" s="179" t="s">
         <v>718</v>
       </c>
-      <c r="B10" s="175"/>
+      <c r="B10" s="180"/>
       <c r="C10" s="7" t="s">
         <v>860</v>
       </c>
@@ -26941,10 +26941,10 @@
       <c r="F16" s="58"/>
     </row>
     <row r="17" spans="1:6" ht="28.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="174" t="s">
+      <c r="A17" s="179" t="s">
         <v>732</v>
       </c>
-      <c r="B17" s="175"/>
+      <c r="B17" s="180"/>
       <c r="C17" s="7" t="s">
         <v>862</v>
       </c>
@@ -27163,10 +27163,10 @@
       <c r="F28" s="58"/>
     </row>
     <row r="29" spans="1:6" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="176" t="s">
+      <c r="A29" s="181" t="s">
         <v>733</v>
       </c>
-      <c r="B29" s="177"/>
+      <c r="B29" s="182"/>
       <c r="C29" s="7" t="s">
         <v>886</v>
       </c>
@@ -27434,7 +27434,7 @@
       </c>
       <c r="F43" s="58"/>
     </row>
-    <row r="44" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="66" t="s">
         <v>97</v>
       </c>
@@ -27560,7 +27560,7 @@
       </c>
       <c r="F50" s="58"/>
     </row>
-    <row r="51" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="67" t="s">
         <v>218</v>
       </c>
@@ -27632,7 +27632,7 @@
       </c>
       <c r="F54" s="58"/>
     </row>
-    <row r="55" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="66" t="s">
         <v>218</v>
       </c>
@@ -27651,10 +27651,10 @@
       <c r="F55" s="58"/>
     </row>
     <row r="56" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="174" t="s">
+      <c r="A56" s="179" t="s">
         <v>113</v>
       </c>
-      <c r="B56" s="175"/>
+      <c r="B56" s="180"/>
       <c r="C56" s="7" t="s">
         <v>88</v>
       </c>
@@ -27704,7 +27704,7 @@
       </c>
       <c r="F58" s="58"/>
     </row>
-    <row r="59" spans="1:6" ht="69.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:6" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="66" t="s">
         <v>95</v>
       </c>
@@ -27891,10 +27891,10 @@
       <c r="F68" s="58"/>
     </row>
     <row r="69" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="174" t="s">
+      <c r="A69" s="179" t="s">
         <v>135</v>
       </c>
-      <c r="B69" s="175"/>
+      <c r="B69" s="180"/>
       <c r="C69" s="7" t="s">
         <v>88</v>
       </c>
@@ -28053,10 +28053,10 @@
       <c r="F77" s="58"/>
     </row>
     <row r="78" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="174" t="s">
+      <c r="A78" s="179" t="s">
         <v>152</v>
       </c>
-      <c r="B78" s="175"/>
+      <c r="B78" s="180"/>
       <c r="C78" s="7" t="s">
         <v>88</v>
       </c>
@@ -28167,10 +28167,10 @@
       </c>
     </row>
     <row r="84" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A84" s="174" t="s">
+      <c r="A84" s="179" t="s">
         <v>163</v>
       </c>
-      <c r="B84" s="175"/>
+      <c r="B84" s="180"/>
       <c r="C84" s="7" t="s">
         <v>88</v>
       </c>
@@ -28417,10 +28417,10 @@
       <c r="F96" s="58"/>
     </row>
     <row r="97" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A97" s="174" t="s">
+      <c r="A97" s="179" t="s">
         <v>187</v>
       </c>
-      <c r="B97" s="175"/>
+      <c r="B97" s="180"/>
       <c r="C97" s="7" t="s">
         <v>88</v>
       </c>
@@ -28511,10 +28511,10 @@
       <c r="F101" s="58"/>
     </row>
     <row r="102" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A102" s="174" t="s">
+      <c r="A102" s="179" t="s">
         <v>194</v>
       </c>
-      <c r="B102" s="175"/>
+      <c r="B102" s="180"/>
       <c r="C102" s="7" t="s">
         <v>88</v>
       </c>
@@ -28564,7 +28564,7 @@
       </c>
       <c r="F104" s="58"/>
     </row>
-    <row r="105" spans="1:6" ht="138.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:6" ht="152.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A105" s="66" t="s">
         <v>95</v>
       </c>
@@ -28659,10 +28659,10 @@
       </c>
     </row>
     <row r="110" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A110" s="174" t="s">
+      <c r="A110" s="179" t="s">
         <v>205</v>
       </c>
-      <c r="B110" s="175"/>
+      <c r="B110" s="180"/>
       <c r="C110" s="7" t="s">
         <v>88</v>
       </c>
@@ -28731,10 +28731,10 @@
       <c r="F113" s="58"/>
     </row>
     <row r="114" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A114" s="174" t="s">
+      <c r="A114" s="179" t="s">
         <v>212</v>
       </c>
-      <c r="B114" s="175"/>
+      <c r="B114" s="180"/>
       <c r="C114" s="7" t="s">
         <v>88</v>
       </c>
@@ -28803,10 +28803,10 @@
       <c r="F117" s="58"/>
     </row>
     <row r="118" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A118" s="174" t="s">
+      <c r="A118" s="179" t="s">
         <v>219</v>
       </c>
-      <c r="B118" s="175"/>
+      <c r="B118" s="180"/>
       <c r="C118" s="7" t="s">
         <v>816</v>
       </c>
@@ -28966,11 +28966,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="C2:C9"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A56:B56"/>
     <mergeCell ref="A110:B110"/>
     <mergeCell ref="A114:B114"/>
     <mergeCell ref="A118:B118"/>
@@ -28980,6 +28975,11 @@
     <mergeCell ref="A84:B84"/>
     <mergeCell ref="A97:B97"/>
     <mergeCell ref="A102:B102"/>
+    <mergeCell ref="C2:C9"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A56:B56"/>
   </mergeCells>
   <conditionalFormatting sqref="A10 A33:A37 A39:A41 A109:A251 A14:A31 A95:A107 A56:A80 A82:A87">
     <cfRule type="beginsWith" dxfId="1417" priority="354" stopIfTrue="1" operator="beginsWith" text="Innovative">
@@ -29832,7 +29832,7 @@
       <c r="B2" s="58" t="s">
         <v>74</v>
       </c>
-      <c r="C2" s="178" t="s">
+      <c r="C2" s="174" t="s">
         <v>854</v>
       </c>
       <c r="D2" s="64">
@@ -29855,7 +29855,7 @@
       <c r="B3" s="58" t="s">
         <v>76</v>
       </c>
-      <c r="C3" s="179"/>
+      <c r="C3" s="175"/>
       <c r="D3" s="64">
         <f>SUMPRODUCT(($A$10:$A$241="Basic")*(D$10:D$241="Missing"))+0.5*SUMPRODUCT(($A$10:$A$241="Basic")*(D$10:D$241="Partial"))</f>
         <v>0</v>
@@ -29876,7 +29876,7 @@
       <c r="B4" s="58" t="s">
         <v>78</v>
       </c>
-      <c r="C4" s="179"/>
+      <c r="C4" s="175"/>
       <c r="D4" s="64">
         <f>SUMPRODUCT(($A$10:$A$241="Intermediate")*(D$10:D$241="Missing"))+0.5*SUMPRODUCT(($A$10:$A$241="Intermediate")*(D$10:D$241="Partial"))</f>
         <v>0</v>
@@ -29897,7 +29897,7 @@
       <c r="B5" s="58" t="s">
         <v>80</v>
       </c>
-      <c r="C5" s="179"/>
+      <c r="C5" s="175"/>
       <c r="D5" s="64">
         <f>SUMPRODUCT(($A$10:$A$241="Intermediate")*(D$10:D$241="Completed"))+SUMPRODUCT(($A$10:$A$241="Intermediate")*(D$10:D$241="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$241="Intermediate")*(D$10:D$241="Partial"))</f>
         <v>6</v>
@@ -29918,7 +29918,7 @@
       <c r="B6" s="58" t="s">
         <v>82</v>
       </c>
-      <c r="C6" s="179"/>
+      <c r="C6" s="175"/>
       <c r="D6" s="64">
         <f>SUMPRODUCT(($A$10:$A$241="Advanced")*(D$10:D$241="Missing"))+0.5*SUMPRODUCT(($A$10:$A$241="Advanced")*(D$10:D$241="Partial"))</f>
         <v>10</v>
@@ -29939,7 +29939,7 @@
       <c r="B7" s="58" t="s">
         <v>84</v>
       </c>
-      <c r="C7" s="179"/>
+      <c r="C7" s="175"/>
       <c r="D7" s="64">
         <f>SUMPRODUCT(($A$10:$A$241="Advanced")*(D$10:D$241="Completed"))+SUMPRODUCT(($A$10:$A$241="Advanced")*(D$10:D$241="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$241="Advanced")*(D$10:D$241="Partial"))</f>
         <v>2</v>
@@ -29960,7 +29960,7 @@
       <c r="B8" s="58" t="s">
         <v>86</v>
       </c>
-      <c r="C8" s="179"/>
+      <c r="C8" s="175"/>
       <c r="D8" s="64">
         <f>SUMPRODUCT(($A$10:$A$241="Professional")*(D$10:D$241="Completed"))+SUMPRODUCT(($A$10:$A$241="Professional")*(D$10:D$241="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$241="Professional")*(D$10:D$241="Partial"))</f>
         <v>1</v>
@@ -29975,11 +29975,11 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="181" t="s">
+      <c r="A9" s="177" t="s">
         <v>87</v>
       </c>
-      <c r="B9" s="182"/>
-      <c r="C9" s="180"/>
+      <c r="B9" s="178"/>
+      <c r="C9" s="176"/>
       <c r="D9" s="64">
         <f>SUMPRODUCT(($A$10:$A$241="Innovative")*(D$10:D$241="Completed"))+SUMPRODUCT(($A$10:$A$241="Innovative")*(D$10:D$241="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$241="Innovative")*(D$10:D$241="Partial"))</f>
         <v>2</v>
@@ -29994,10 +29994,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="174" t="s">
+      <c r="A10" s="179" t="s">
         <v>803</v>
       </c>
-      <c r="B10" s="175"/>
+      <c r="B10" s="180"/>
       <c r="C10" s="7" t="s">
         <v>855</v>
       </c>
@@ -30084,10 +30084,10 @@
       <c r="F14" s="58"/>
     </row>
     <row r="15" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="174" t="s">
+      <c r="A15" s="179" t="s">
         <v>249</v>
       </c>
-      <c r="B15" s="175"/>
+      <c r="B15" s="180"/>
       <c r="C15" s="7" t="s">
         <v>88</v>
       </c>
@@ -30236,10 +30236,10 @@
       <c r="F22" s="58"/>
     </row>
     <row r="23" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="174" t="s">
+      <c r="A23" s="179" t="s">
         <v>257</v>
       </c>
-      <c r="B23" s="175"/>
+      <c r="B23" s="180"/>
       <c r="C23" s="7" t="s">
         <v>88</v>
       </c>
@@ -30384,10 +30384,10 @@
       <c r="F30" s="58"/>
     </row>
     <row r="31" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="174" t="s">
+      <c r="A31" s="179" t="s">
         <v>262</v>
       </c>
-      <c r="B31" s="175"/>
+      <c r="B31" s="180"/>
       <c r="C31" s="7" t="s">
         <v>88</v>
       </c>
@@ -30870,10 +30870,10 @@
       <c r="F56" s="58"/>
     </row>
     <row r="57" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="174" t="s">
+      <c r="A57" s="179" t="s">
         <v>288</v>
       </c>
-      <c r="B57" s="175"/>
+      <c r="B57" s="180"/>
       <c r="C57" s="71" t="s">
         <v>825</v>
       </c>
@@ -31093,7 +31093,7 @@
         <v>875</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A69" s="117" t="s">
         <v>134</v>
       </c>
@@ -31272,10 +31272,10 @@
       <c r="F77" s="58"/>
     </row>
     <row r="78" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="174" t="s">
+      <c r="A78" s="179" t="s">
         <v>299</v>
       </c>
-      <c r="B78" s="175"/>
+      <c r="B78" s="180"/>
       <c r="C78" s="7" t="s">
         <v>88</v>
       </c>
@@ -33205,7 +33205,7 @@
       <c r="B2" s="58" t="s">
         <v>74</v>
       </c>
-      <c r="C2" s="178" t="s">
+      <c r="C2" s="174" t="s">
         <v>823</v>
       </c>
       <c r="D2" s="64">
@@ -33228,7 +33228,7 @@
       <c r="B3" s="58" t="s">
         <v>76</v>
       </c>
-      <c r="C3" s="179"/>
+      <c r="C3" s="175"/>
       <c r="D3" s="64">
         <f>SUMPRODUCT(($A$10:$A$177="Basic")*(D$10:D$177="Missing"))+0.5*SUMPRODUCT(($A$10:$A$177="Basic")*(D$10:D$177="Partial"))</f>
         <v>0</v>
@@ -33249,7 +33249,7 @@
       <c r="B4" s="58" t="s">
         <v>78</v>
       </c>
-      <c r="C4" s="179"/>
+      <c r="C4" s="175"/>
       <c r="D4" s="64">
         <f>SUMPRODUCT(($A$10:$A$177="Intermediate")*(D$10:D$177="Missing"))+0.5*SUMPRODUCT(($A$10:$A$177="Intermediate")*(D$10:D$177="Partial"))</f>
         <v>0</v>
@@ -33270,7 +33270,7 @@
       <c r="B5" s="58" t="s">
         <v>80</v>
       </c>
-      <c r="C5" s="179"/>
+      <c r="C5" s="175"/>
       <c r="D5" s="64">
         <f>SUMPRODUCT(($A$10:$A$177="Intermediate")*(D$10:D$177="Completed"))+SUMPRODUCT(($A$10:$A$177="Intermediate")*(D$10:D$177="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$177="Intermediate")*(D$10:D$177="Partial"))</f>
         <v>5</v>
@@ -33291,7 +33291,7 @@
       <c r="B6" s="58" t="s">
         <v>82</v>
       </c>
-      <c r="C6" s="179"/>
+      <c r="C6" s="175"/>
       <c r="D6" s="64">
         <f>SUMPRODUCT(($A$10:$A$177="Advanced")*(D$10:D$177="Missing"))+0.5*SUMPRODUCT(($A$10:$A$177="Advanced")*(D$10:D$177="Partial"))</f>
         <v>5.5</v>
@@ -33312,7 +33312,7 @@
       <c r="B7" s="58" t="s">
         <v>84</v>
       </c>
-      <c r="C7" s="179"/>
+      <c r="C7" s="175"/>
       <c r="D7" s="64">
         <f>SUMPRODUCT(($A$10:$A$177="Advanced")*(D$10:D$177="Completed"))+SUMPRODUCT(($A$10:$A$177="Advanced")*(D$10:D$177="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$177="Advanced")*(D$10:D$177="Partial"))</f>
         <v>1.5</v>
@@ -33333,7 +33333,7 @@
       <c r="B8" s="58" t="s">
         <v>86</v>
       </c>
-      <c r="C8" s="179"/>
+      <c r="C8" s="175"/>
       <c r="D8" s="64">
         <f>SUMPRODUCT(($A$10:$A$177="Professional")*(D$10:D$177="Completed"))+SUMPRODUCT(($A$10:$A$177="Professional")*(D$10:D$177="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$177="Professional")*(D$10:D$177="Partial"))</f>
         <v>0</v>
@@ -33348,11 +33348,11 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="181" t="s">
+      <c r="A9" s="177" t="s">
         <v>87</v>
       </c>
-      <c r="B9" s="182"/>
-      <c r="C9" s="180"/>
+      <c r="B9" s="178"/>
+      <c r="C9" s="176"/>
       <c r="D9" s="64">
         <f>SUMPRODUCT(($A$10:$A$177="Innovative")*(D$10:D$177="Completed"))+SUMPRODUCT(($A$10:$A$177="Innovative")*(D$10:D$177="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$177="Innovative")*(D$10:D$177="Partial"))</f>
         <v>0</v>
@@ -33367,10 +33367,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="174" t="s">
+      <c r="A10" s="179" t="s">
         <v>237</v>
       </c>
-      <c r="B10" s="175"/>
+      <c r="B10" s="180"/>
       <c r="C10" s="7" t="s">
         <v>88</v>
       </c>
@@ -33595,10 +33595,10 @@
       <c r="F21" s="58"/>
     </row>
     <row r="22" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="174" t="s">
+      <c r="A22" s="179" t="s">
         <v>528</v>
       </c>
-      <c r="B22" s="175"/>
+      <c r="B22" s="180"/>
       <c r="C22" s="7" t="s">
         <v>88</v>
       </c>
@@ -33757,10 +33757,10 @@
       <c r="F30" s="58"/>
     </row>
     <row r="31" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="174" t="s">
+      <c r="A31" s="179" t="s">
         <v>544</v>
       </c>
-      <c r="B31" s="175"/>
+      <c r="B31" s="180"/>
       <c r="C31" s="7" t="s">
         <v>88</v>
       </c>
@@ -33983,10 +33983,10 @@
       <c r="F42" s="58"/>
     </row>
     <row r="43" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="174" t="s">
+      <c r="A43" s="179" t="s">
         <v>655</v>
       </c>
-      <c r="B43" s="175"/>
+      <c r="B43" s="180"/>
       <c r="C43" s="7" t="s">
         <v>88</v>
       </c>
@@ -34317,7 +34317,7 @@
       <c r="B2" s="58" t="s">
         <v>74</v>
       </c>
-      <c r="C2" s="178" t="s">
+      <c r="C2" s="174" t="s">
         <v>379</v>
       </c>
       <c r="D2" s="64">
@@ -34340,7 +34340,7 @@
       <c r="B3" s="58" t="s">
         <v>76</v>
       </c>
-      <c r="C3" s="179"/>
+      <c r="C3" s="175"/>
       <c r="D3" s="64">
         <f>SUMPRODUCT(($A$10:$A$248="Basic")*(D$10:D$248="Missing"))+0.5*SUMPRODUCT(($A$10:$A$248="Basic")*(D$10:D$248="Partial"))</f>
         <v>0</v>
@@ -34361,7 +34361,7 @@
       <c r="B4" s="58" t="s">
         <v>78</v>
       </c>
-      <c r="C4" s="179"/>
+      <c r="C4" s="175"/>
       <c r="D4" s="64">
         <f>SUMPRODUCT(($A$10:$A$248="Intermediate")*(D$10:D$248="Missing"))+0.5*SUMPRODUCT(($A$10:$A$248="Intermediate")*(D$10:D$248="Partial"))</f>
         <v>0</v>
@@ -34382,7 +34382,7 @@
       <c r="B5" s="58" t="s">
         <v>80</v>
       </c>
-      <c r="C5" s="179"/>
+      <c r="C5" s="175"/>
       <c r="D5" s="64">
         <f>SUMPRODUCT(($A$10:$A$248="Intermediate")*(D$10:D$248="Completed"))+SUMPRODUCT(($A$10:$A$248="Intermediate")*(D$10:D$248="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$248="Intermediate")*(D$10:D$248="Partial"))</f>
         <v>1</v>
@@ -34403,7 +34403,7 @@
       <c r="B6" s="58" t="s">
         <v>82</v>
       </c>
-      <c r="C6" s="179"/>
+      <c r="C6" s="175"/>
       <c r="D6" s="64">
         <f>SUMPRODUCT(($A$10:$A$248="Advanced")*(D$10:D$248="Missing"))+0.5*SUMPRODUCT(($A$10:$A$248="Advanced")*(D$10:D$248="Partial"))</f>
         <v>0</v>
@@ -34424,7 +34424,7 @@
       <c r="B7" s="58" t="s">
         <v>84</v>
       </c>
-      <c r="C7" s="179"/>
+      <c r="C7" s="175"/>
       <c r="D7" s="64">
         <f>SUMPRODUCT(($A$10:$A$248="Advanced")*(D$10:D$248="Completed"))+SUMPRODUCT(($A$10:$A$248="Advanced")*(D$10:D$248="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$248="Advanced")*(D$10:D$248="Partial"))</f>
         <v>2</v>
@@ -34445,7 +34445,7 @@
       <c r="B8" s="58" t="s">
         <v>86</v>
       </c>
-      <c r="C8" s="179"/>
+      <c r="C8" s="175"/>
       <c r="D8" s="64">
         <f>SUMPRODUCT(($A$10:$A$248="Professional")*(D$10:D$248="Completed"))+SUMPRODUCT(($A$10:$A$248="Professional")*(D$10:D$248="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$248="Professional")*(D$10:D$248="Partial"))</f>
         <v>0</v>
@@ -34460,11 +34460,11 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="181" t="s">
+      <c r="A9" s="177" t="s">
         <v>87</v>
       </c>
-      <c r="B9" s="182"/>
-      <c r="C9" s="180"/>
+      <c r="B9" s="178"/>
+      <c r="C9" s="176"/>
       <c r="D9" s="64">
         <f>SUMPRODUCT(($A$10:$A$248="Innovative")*(D$10:D$248="Completed"))+SUMPRODUCT(($A$10:$A$248="Innovative")*(D$10:D$248="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$248="Innovative")*(D$10:D$248="Partial"))</f>
         <v>1</v>
@@ -34479,10 +34479,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="174" t="s">
+      <c r="A10" s="179" t="s">
         <v>380</v>
       </c>
-      <c r="B10" s="175"/>
+      <c r="B10" s="180"/>
       <c r="C10" s="7" t="s">
         <v>88</v>
       </c>
@@ -34591,10 +34591,10 @@
       <c r="F15" s="58"/>
     </row>
     <row r="16" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="174" t="s">
+      <c r="A16" s="179" t="s">
         <v>391</v>
       </c>
-      <c r="B16" s="175"/>
+      <c r="B16" s="180"/>
       <c r="C16" s="7" t="s">
         <v>88</v>
       </c>
@@ -34699,10 +34699,10 @@
       <c r="F21" s="58"/>
     </row>
     <row r="22" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="174" t="s">
+      <c r="A22" s="179" t="s">
         <v>402</v>
       </c>
-      <c r="B22" s="175"/>
+      <c r="B22" s="180"/>
       <c r="C22" s="7" t="s">
         <v>819</v>
       </c>
@@ -34825,10 +34825,10 @@
       <c r="F28" s="58"/>
     </row>
     <row r="29" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="174" t="s">
+      <c r="A29" s="179" t="s">
         <v>415</v>
       </c>
-      <c r="B29" s="175"/>
+      <c r="B29" s="180"/>
       <c r="C29" s="7" t="s">
         <v>817</v>
       </c>
@@ -34971,10 +34971,10 @@
       <c r="F36" s="58"/>
     </row>
     <row r="37" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="174" t="s">
+      <c r="A37" s="179" t="s">
         <v>430</v>
       </c>
-      <c r="B37" s="175"/>
+      <c r="B37" s="180"/>
       <c r="C37" s="7" t="s">
         <v>818</v>
       </c>
@@ -35097,10 +35097,10 @@
       <c r="F43" s="58"/>
     </row>
     <row r="44" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="174" t="s">
+      <c r="A44" s="179" t="s">
         <v>443</v>
       </c>
-      <c r="B44" s="175"/>
+      <c r="B44" s="180"/>
       <c r="C44" s="7" t="s">
         <v>88</v>
       </c>
@@ -36283,7 +36283,7 @@
       <c r="B2" s="58" t="s">
         <v>74</v>
       </c>
-      <c r="C2" s="178" t="s">
+      <c r="C2" s="174" t="s">
         <v>468</v>
       </c>
       <c r="D2" s="64">
@@ -36306,7 +36306,7 @@
       <c r="B3" s="58" t="s">
         <v>76</v>
       </c>
-      <c r="C3" s="179"/>
+      <c r="C3" s="175"/>
       <c r="D3" s="64">
         <f>SUMPRODUCT(($A$10:$A$227="Basic")*(D$10:D$227="Missing"))+0.5*SUMPRODUCT(($A$10:$A$227="Basic")*(D$10:D$227="Partial"))</f>
         <v>0</v>
@@ -36327,7 +36327,7 @@
       <c r="B4" s="58" t="s">
         <v>78</v>
       </c>
-      <c r="C4" s="179"/>
+      <c r="C4" s="175"/>
       <c r="D4" s="64">
         <f>SUMPRODUCT(($A$10:$A$227="Intermediate")*(D$10:D$227="Missing"))+0.5*SUMPRODUCT(($A$10:$A$227="Intermediate")*(D$10:D$227="Partial"))</f>
         <v>0</v>
@@ -36348,7 +36348,7 @@
       <c r="B5" s="58" t="s">
         <v>80</v>
       </c>
-      <c r="C5" s="179"/>
+      <c r="C5" s="175"/>
       <c r="D5" s="64">
         <f>SUMPRODUCT(($A$10:$A$227="Intermediate")*(D$10:D$227="Completed"))+SUMPRODUCT(($A$10:$A$227="Intermediate")*(D$10:D$227="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$227="Intermediate")*(D$10:D$227="Partial"))</f>
         <v>6</v>
@@ -36369,7 +36369,7 @@
       <c r="B6" s="58" t="s">
         <v>82</v>
       </c>
-      <c r="C6" s="179"/>
+      <c r="C6" s="175"/>
       <c r="D6" s="64">
         <f>SUMPRODUCT(($A$10:$A$227="Advanced")*(D$10:D$227="Missing"))+0.5*SUMPRODUCT(($A$10:$A$227="Advanced")*(D$10:D$227="Partial"))</f>
         <v>3</v>
@@ -36390,7 +36390,7 @@
       <c r="B7" s="58" t="s">
         <v>84</v>
       </c>
-      <c r="C7" s="179"/>
+      <c r="C7" s="175"/>
       <c r="D7" s="64">
         <f>SUMPRODUCT(($A$10:$A$227="Advanced")*(D$10:D$227="Completed"))+SUMPRODUCT(($A$10:$A$227="Advanced")*(D$10:D$227="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$227="Advanced")*(D$10:D$227="Partial"))</f>
         <v>6</v>
@@ -36411,7 +36411,7 @@
       <c r="B8" s="58" t="s">
         <v>86</v>
       </c>
-      <c r="C8" s="179"/>
+      <c r="C8" s="175"/>
       <c r="D8" s="64">
         <f>SUMPRODUCT(($A$10:$A$227="Professional")*(D$10:D$227="Completed"))+SUMPRODUCT(($A$10:$A$227="Professional")*(D$10:D$227="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$227="Professional")*(D$10:D$227="Partial"))</f>
         <v>2</v>
@@ -36426,11 +36426,11 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="181" t="s">
+      <c r="A9" s="177" t="s">
         <v>87</v>
       </c>
-      <c r="B9" s="182"/>
-      <c r="C9" s="180"/>
+      <c r="B9" s="178"/>
+      <c r="C9" s="176"/>
       <c r="D9" s="64">
         <f>SUMPRODUCT(($A$10:$A$227="Innovative")*(D$10:D$227="Completed"))+SUMPRODUCT(($A$10:$A$227="Innovative")*(D$10:D$227="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$227="Innovative")*(D$10:D$227="Partial"))</f>
         <v>0</v>
@@ -36445,10 +36445,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="174" t="s">
+      <c r="A10" s="179" t="s">
         <v>469</v>
       </c>
-      <c r="B10" s="175"/>
+      <c r="B10" s="180"/>
       <c r="C10" s="7" t="s">
         <v>88</v>
       </c>
@@ -36809,10 +36809,10 @@
       <c r="F28" s="58"/>
     </row>
     <row r="29" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="174" t="s">
+      <c r="A29" s="179" t="s">
         <v>505</v>
       </c>
-      <c r="B29" s="175"/>
+      <c r="B29" s="180"/>
       <c r="C29" s="7" t="s">
         <v>814</v>
       </c>
@@ -37029,10 +37029,10 @@
       <c r="F40" s="58"/>
     </row>
     <row r="41" spans="1:6" s="25" customFormat="1" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="174" t="s">
+      <c r="A41" s="179" t="s">
         <v>113</v>
       </c>
-      <c r="B41" s="175"/>
+      <c r="B41" s="180"/>
       <c r="C41" s="7" t="s">
         <v>88</v>
       </c>
@@ -37193,10 +37193,10 @@
       <c r="F49" s="58"/>
     </row>
     <row r="50" spans="1:6" s="25" customFormat="1" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="174" t="s">
+      <c r="A50" s="179" t="s">
         <v>583</v>
       </c>
-      <c r="B50" s="175"/>
+      <c r="B50" s="180"/>
       <c r="C50" s="71" t="s">
         <v>815</v>
       </c>
@@ -38188,7 +38188,7 @@
       <c r="B2" s="58" t="s">
         <v>74</v>
       </c>
-      <c r="C2" s="178" t="s">
+      <c r="C2" s="174" t="s">
         <v>604</v>
       </c>
       <c r="D2" s="64">
@@ -38211,7 +38211,7 @@
       <c r="B3" s="58" t="s">
         <v>76</v>
       </c>
-      <c r="C3" s="179"/>
+      <c r="C3" s="175"/>
       <c r="D3" s="64">
         <f>SUMPRODUCT(($A$10:$A$240="Basic")*(D$10:D$240="Missing"))+0.5*SUMPRODUCT(($A$10:$A$240="Basic")*(D$10:D$240="Partial"))</f>
         <v>0</v>
@@ -38232,7 +38232,7 @@
       <c r="B4" s="58" t="s">
         <v>78</v>
       </c>
-      <c r="C4" s="179"/>
+      <c r="C4" s="175"/>
       <c r="D4" s="64">
         <f>SUMPRODUCT(($A$10:$A$240="Intermediate")*(D$10:D$240="Missing"))+0.5*SUMPRODUCT(($A$10:$A$240="Intermediate")*(D$10:D$240="Partial"))</f>
         <v>0</v>
@@ -38253,7 +38253,7 @@
       <c r="B5" s="58" t="s">
         <v>80</v>
       </c>
-      <c r="C5" s="179"/>
+      <c r="C5" s="175"/>
       <c r="D5" s="64">
         <f>SUMPRODUCT(($A$10:$A$240="Intermediate")*(D$10:D$240="Completed"))+SUMPRODUCT(($A$10:$A$240="Intermediate")*(D$10:D$240="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$240="Intermediate")*(D$10:D$240="Partial"))</f>
         <v>3</v>
@@ -38274,7 +38274,7 @@
       <c r="B6" s="58" t="s">
         <v>82</v>
       </c>
-      <c r="C6" s="179"/>
+      <c r="C6" s="175"/>
       <c r="D6" s="64">
         <f>SUMPRODUCT(($A$10:$A$240="Advanced")*(D$10:D$240="Missing"))+0.5*SUMPRODUCT(($A$10:$A$240="Advanced")*(D$10:D$240="Partial"))</f>
         <v>1</v>
@@ -38295,7 +38295,7 @@
       <c r="B7" s="58" t="s">
         <v>84</v>
       </c>
-      <c r="C7" s="179"/>
+      <c r="C7" s="175"/>
       <c r="D7" s="64">
         <f>SUMPRODUCT(($A$10:$A$240="Advanced")*(D$10:D$240="Completed"))+SUMPRODUCT(($A$10:$A$240="Advanced")*(D$10:D$240="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$240="Advanced")*(D$10:D$240="Partial"))</f>
         <v>7</v>
@@ -38316,7 +38316,7 @@
       <c r="B8" s="58" t="s">
         <v>86</v>
       </c>
-      <c r="C8" s="179"/>
+      <c r="C8" s="175"/>
       <c r="D8" s="64">
         <f>SUMPRODUCT(($A$10:$A$240="Professional")*(D$10:D$240="Completed"))+SUMPRODUCT(($A$10:$A$240="Professional")*(D$10:D$240="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$240="Professional")*(D$10:D$240="Partial"))</f>
         <v>4</v>
@@ -38331,11 +38331,11 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="181" t="s">
+      <c r="A9" s="177" t="s">
         <v>87</v>
       </c>
-      <c r="B9" s="182"/>
-      <c r="C9" s="180"/>
+      <c r="B9" s="178"/>
+      <c r="C9" s="176"/>
       <c r="D9" s="64">
         <f>SUMPRODUCT(($A$10:$A$240="Innovative")*(D$10:D$240="Completed"))+SUMPRODUCT(($A$10:$A$240="Innovative")*(D$10:D$240="Pre-Passed"))+0.5*SUMPRODUCT(($A$10:$A$240="Innovative")*(D$10:D$240="Partial"))</f>
         <v>3</v>
@@ -38350,10 +38350,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="174" t="s">
+      <c r="A10" s="179" t="s">
         <v>605</v>
       </c>
-      <c r="B10" s="175"/>
+      <c r="B10" s="180"/>
       <c r="C10" s="71" t="s">
         <v>808</v>
       </c>
@@ -38572,10 +38572,10 @@
       <c r="F21" s="58"/>
     </row>
     <row r="22" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="174" t="s">
+      <c r="A22" s="179" t="s">
         <v>628</v>
       </c>
-      <c r="B22" s="175"/>
+      <c r="B22" s="180"/>
       <c r="C22" s="7" t="s">
         <v>88</v>
       </c>
@@ -38790,10 +38790,10 @@
       <c r="F33" s="58"/>
     </row>
     <row r="34" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="174" t="s">
+      <c r="A34" s="179" t="s">
         <v>804</v>
       </c>
-      <c r="B34" s="175"/>
+      <c r="B34" s="180"/>
       <c r="C34" s="7" t="s">
         <v>809</v>
       </c>
@@ -38918,10 +38918,10 @@
       <c r="F40" s="58"/>
     </row>
     <row r="41" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="174" t="s">
+      <c r="A41" s="179" t="s">
         <v>674</v>
       </c>
-      <c r="B41" s="175"/>
+      <c r="B41" s="180"/>
       <c r="C41" s="7" t="s">
         <v>88</v>
       </c>
@@ -39848,65 +39848,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="183" t="s">
+      <c r="A1" s="193" t="s">
         <v>699</v>
       </c>
       <c r="B1" s="73"/>
-      <c r="C1" s="198" t="s">
+      <c r="C1" s="183" t="s">
         <v>683</v>
       </c>
-      <c r="D1" s="199"/>
-      <c r="E1" s="198" t="s">
+      <c r="D1" s="184"/>
+      <c r="E1" s="183" t="s">
         <v>684</v>
       </c>
-      <c r="F1" s="199"/>
-      <c r="G1" s="198" t="s">
+      <c r="F1" s="184"/>
+      <c r="G1" s="183" t="s">
         <v>685</v>
       </c>
-      <c r="H1" s="199"/>
+      <c r="H1" s="184"/>
     </row>
     <row r="2" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="184"/>
+      <c r="A2" s="194"/>
       <c r="B2" s="73"/>
-      <c r="C2" s="200" t="s">
+      <c r="C2" s="185" t="s">
         <v>682</v>
       </c>
-      <c r="D2" s="201"/>
-      <c r="E2" s="200" t="s">
+      <c r="D2" s="186"/>
+      <c r="E2" s="185" t="s">
         <v>682</v>
       </c>
-      <c r="F2" s="201"/>
-      <c r="G2" s="200" t="s">
+      <c r="F2" s="186"/>
+      <c r="G2" s="185" t="s">
         <v>682</v>
       </c>
-      <c r="H2" s="201"/>
-      <c r="J2" s="186" t="s">
+      <c r="H2" s="186"/>
+      <c r="J2" s="196" t="s">
         <v>701</v>
       </c>
-      <c r="K2" s="187"/>
-      <c r="L2" s="188"/>
+      <c r="K2" s="197"/>
+      <c r="L2" s="198"/>
     </row>
     <row r="3" spans="1:12" ht="22.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="185"/>
+      <c r="A3" s="195"/>
       <c r="B3" s="74"/>
-      <c r="C3" s="196">
+      <c r="C3" s="187">
         <f>MAX(0,MIN(1,IF((A6+C6) &lt;= 0.95, ROUND(A6+C6,2), FLOOR((0.95+(A6+C6-0.95)/5),0.01))))</f>
         <v>0.95</v>
       </c>
-      <c r="D3" s="197"/>
-      <c r="E3" s="196">
+      <c r="D3" s="188"/>
+      <c r="E3" s="187">
         <f>MAX(0,MIN(1,IF((A6+E6) &lt;= 0.95, ROUND(A6+E6,2), FLOOR((0.95+(A6+E6-0.95)/5),0.01))))</f>
         <v>0.95</v>
       </c>
-      <c r="F3" s="197"/>
-      <c r="G3" s="196">
+      <c r="F3" s="188"/>
+      <c r="G3" s="187">
         <f>MAX(0,MIN(1,IF((A6+G6) &lt;= 0.95, ROUND(A6+G6,2), FLOOR((0.95+(A6+G6-0.95)/5),0.01))))</f>
         <v>0.95</v>
       </c>
-      <c r="H3" s="197"/>
-      <c r="J3" s="189"/>
-      <c r="K3" s="190"/>
-      <c r="L3" s="191"/>
+      <c r="H3" s="188"/>
+      <c r="J3" s="199"/>
+      <c r="K3" s="200"/>
+      <c r="L3" s="201"/>
     </row>
     <row r="4" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
@@ -39923,19 +39923,19 @@
         <v>686</v>
       </c>
       <c r="B5" s="10"/>
-      <c r="C5" s="147" t="s">
+      <c r="C5" s="120" t="s">
         <v>687</v>
       </c>
-      <c r="D5" s="149"/>
-      <c r="E5" s="147" t="s">
+      <c r="D5" s="122"/>
+      <c r="E5" s="120" t="s">
         <v>688</v>
       </c>
-      <c r="F5" s="149"/>
-      <c r="G5" s="147" t="s">
+      <c r="F5" s="122"/>
+      <c r="G5" s="120" t="s">
         <v>689</v>
       </c>
-      <c r="H5" s="149"/>
-      <c r="J5" s="141" t="s">
+      <c r="H5" s="122"/>
+      <c r="J5" s="129" t="s">
         <v>715</v>
       </c>
       <c r="K5" s="30"/>
@@ -39949,22 +39949,22 @@
         <v>0.71</v>
       </c>
       <c r="B6" s="10"/>
-      <c r="C6" s="193">
+      <c r="C6" s="190">
         <f>D15+D24+D33+D42+D51+D60</f>
         <v>0.24000000000000002</v>
       </c>
-      <c r="D6" s="194"/>
-      <c r="E6" s="193">
+      <c r="D6" s="191"/>
+      <c r="E6" s="190">
         <f>F15+F24+F33+F42+F51+F60</f>
         <v>0.24000000000000002</v>
       </c>
-      <c r="F6" s="194"/>
-      <c r="G6" s="193">
+      <c r="F6" s="191"/>
+      <c r="G6" s="190">
         <f>H15+H24+H33+H42+H51+H60</f>
         <v>0.24000000000000002</v>
       </c>
-      <c r="H6" s="194"/>
-      <c r="J6" s="142"/>
+      <c r="H6" s="191"/>
+      <c r="J6" s="130"/>
       <c r="K6" s="30"/>
       <c r="L6" s="102" t="s">
         <v>708</v>
@@ -39973,19 +39973,19 @@
     <row r="7" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
       <c r="B7" s="10"/>
-      <c r="C7" s="195" t="s">
+      <c r="C7" s="192" t="s">
         <v>690</v>
       </c>
-      <c r="D7" s="195"/>
-      <c r="E7" s="195" t="s">
+      <c r="D7" s="192"/>
+      <c r="E7" s="192" t="s">
         <v>691</v>
       </c>
-      <c r="F7" s="195"/>
-      <c r="G7" s="195" t="s">
+      <c r="F7" s="192"/>
+      <c r="G7" s="192" t="s">
         <v>692</v>
       </c>
-      <c r="H7" s="195"/>
-      <c r="J7" s="142"/>
+      <c r="H7" s="192"/>
+      <c r="J7" s="130"/>
       <c r="K7" s="103"/>
       <c r="L7" s="102" t="s">
         <v>709</v>
@@ -40016,7 +40016,7 @@
       <c r="H8" s="85" t="s">
         <v>33</v>
       </c>
-      <c r="J8" s="142"/>
+      <c r="J8" s="130"/>
       <c r="K8" s="103"/>
       <c r="L8" s="102" t="s">
         <v>710</v>
@@ -40052,7 +40052,7 @@
         <f>B9*G9</f>
         <v>0</v>
       </c>
-      <c r="J9" s="142"/>
+      <c r="J9" s="130"/>
       <c r="K9" s="103"/>
       <c r="L9" s="102" t="s">
         <v>711</v>
@@ -40088,7 +40088,7 @@
         <f t="shared" ref="H10:H14" si="2">B10*G10</f>
         <v>0</v>
       </c>
-      <c r="J10" s="142"/>
+      <c r="J10" s="130"/>
       <c r="K10" s="103"/>
       <c r="L10" s="102" t="s">
         <v>712</v>
@@ -40124,7 +40124,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J11" s="142"/>
+      <c r="J11" s="130"/>
       <c r="K11" s="103"/>
       <c r="L11" s="102" t="s">
         <v>713</v>
@@ -40160,7 +40160,7 @@
         <f t="shared" si="2"/>
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="J12" s="143"/>
+      <c r="J12" s="131"/>
       <c r="K12" s="103"/>
       <c r="L12" s="101" t="s">
         <v>714</v>
@@ -40256,18 +40256,18 @@
     <row r="16" spans="1:12" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
       <c r="B16" s="10"/>
-      <c r="C16" s="192" t="s">
+      <c r="C16" s="189" t="s">
         <v>690</v>
       </c>
-      <c r="D16" s="192"/>
-      <c r="E16" s="192" t="s">
+      <c r="D16" s="189"/>
+      <c r="E16" s="189" t="s">
         <v>691</v>
       </c>
-      <c r="F16" s="192"/>
-      <c r="G16" s="192" t="s">
+      <c r="F16" s="189"/>
+      <c r="G16" s="189" t="s">
         <v>692</v>
       </c>
-      <c r="H16" s="192"/>
+      <c r="H16" s="189"/>
     </row>
     <row r="17" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
@@ -40509,18 +40509,18 @@
     <row r="25" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="3"/>
       <c r="B25" s="10"/>
-      <c r="C25" s="192" t="s">
+      <c r="C25" s="189" t="s">
         <v>690</v>
       </c>
-      <c r="D25" s="192"/>
-      <c r="E25" s="192" t="s">
+      <c r="D25" s="189"/>
+      <c r="E25" s="189" t="s">
         <v>691</v>
       </c>
-      <c r="F25" s="192"/>
-      <c r="G25" s="192" t="s">
+      <c r="F25" s="189"/>
+      <c r="G25" s="189" t="s">
         <v>692</v>
       </c>
-      <c r="H25" s="192"/>
+      <c r="H25" s="189"/>
     </row>
     <row r="26" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
@@ -40762,18 +40762,18 @@
     <row r="34" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="3"/>
       <c r="B34" s="10"/>
-      <c r="C34" s="192" t="s">
+      <c r="C34" s="189" t="s">
         <v>690</v>
       </c>
-      <c r="D34" s="192"/>
-      <c r="E34" s="192" t="s">
+      <c r="D34" s="189"/>
+      <c r="E34" s="189" t="s">
         <v>691</v>
       </c>
-      <c r="F34" s="192"/>
-      <c r="G34" s="192" t="s">
+      <c r="F34" s="189"/>
+      <c r="G34" s="189" t="s">
         <v>692</v>
       </c>
-      <c r="H34" s="192"/>
+      <c r="H34" s="189"/>
     </row>
     <row r="35" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
@@ -41015,18 +41015,18 @@
     <row r="43" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="3"/>
       <c r="B43" s="10"/>
-      <c r="C43" s="192" t="s">
+      <c r="C43" s="189" t="s">
         <v>690</v>
       </c>
-      <c r="D43" s="192"/>
-      <c r="E43" s="192" t="s">
+      <c r="D43" s="189"/>
+      <c r="E43" s="189" t="s">
         <v>691</v>
       </c>
-      <c r="F43" s="192"/>
-      <c r="G43" s="192" t="s">
+      <c r="F43" s="189"/>
+      <c r="G43" s="189" t="s">
         <v>692</v>
       </c>
-      <c r="H43" s="192"/>
+      <c r="H43" s="189"/>
     </row>
     <row r="44" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
@@ -41268,18 +41268,18 @@
     <row r="52" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="3"/>
       <c r="B52" s="10"/>
-      <c r="C52" s="192" t="s">
+      <c r="C52" s="189" t="s">
         <v>690</v>
       </c>
-      <c r="D52" s="192"/>
-      <c r="E52" s="192" t="s">
+      <c r="D52" s="189"/>
+      <c r="E52" s="189" t="s">
         <v>691</v>
       </c>
-      <c r="F52" s="192"/>
-      <c r="G52" s="192" t="s">
+      <c r="F52" s="189"/>
+      <c r="G52" s="189" t="s">
         <v>692</v>
       </c>
-      <c r="H52" s="192"/>
+      <c r="H52" s="189"/>
     </row>
     <row r="53" spans="1:8" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
@@ -41520,26 +41520,6 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:H7"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="J2:L3"/>
     <mergeCell ref="J5:J12"/>
@@ -41556,6 +41536,26 @@
     <mergeCell ref="E16:F16"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>